<commit_message>
Started IO processing and GreenREFORM setup
</commit_message>
<xml_diff>
--- a/projects/CGE_Generator/data/A_IOv.xlsx
+++ b/projects/CGE_Generator/data/A_IOv.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="p" sheetId="1" r:id="rId1"/>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +616,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +714,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +971,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>